<commit_message>
Add GFP, AAV results
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matou\Documents\mutagenesis-benchmarks\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F512CBB7-73E1-4883-9F8B-64BB433D1A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4655BDA-598B-458A-AEB0-9022EC9102AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
   <si>
     <t>GFP</t>
   </si>
@@ -115,6 +115,42 @@
   </si>
   <si>
     <t>0.556</t>
+  </si>
+  <si>
+    <t>avGFP</t>
+  </si>
+  <si>
+    <t>TEM</t>
+  </si>
+  <si>
+    <t>E4B</t>
+  </si>
+  <si>
+    <t>AMIE</t>
+  </si>
+  <si>
+    <t>LGK</t>
+  </si>
+  <si>
+    <t>Pab1</t>
+  </si>
+  <si>
+    <t>UBE2I</t>
+  </si>
+  <si>
+    <t>fitness</t>
+  </si>
+  <si>
+    <t>fitness norm</t>
+  </si>
+  <si>
+    <t>diversity</t>
+  </si>
+  <si>
+    <t>novelty</t>
+  </si>
+  <si>
+    <t>n_replaced_scores</t>
   </si>
 </sst>
 </file>
@@ -139,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,8 +187,20 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -238,12 +286,90 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -257,6 +383,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -540,18 +684,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:P6"/>
+  <dimension ref="B2:AD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="2" max="16" width="10.6796875" customWidth="1"/>
+    <col min="19" max="22" width="12.54296875" customWidth="1"/>
+    <col min="23" max="23" width="16.36328125" customWidth="1"/>
+    <col min="26" max="29" width="12.54296875" customWidth="1"/>
+    <col min="30" max="30" width="16.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="2" spans="2:30" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="B2" t="s">
         <v>17</v>
       </c>
@@ -559,7 +707,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="3" spans="2:30" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -596,8 +744,44 @@
       <c r="P3" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="R3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD3" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.75">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.75">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -634,8 +818,24 @@
       <c r="P4" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="R4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="S4" s="11"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="Y4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="9"/>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.75">
+    <row r="5" spans="2:30" x14ac:dyDescent="0.75">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -672,8 +872,24 @@
       <c r="P5" s="6" t="s">
         <v>29</v>
       </c>
+      <c r="R5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="S5" s="12"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="Y5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
     </row>
-    <row r="6" spans="2:16" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="6" spans="2:30" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -710,6 +926,112 @@
       <c r="P6" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="R6" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="S6" s="13"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="Y6" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="8"/>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.75">
+      <c r="R7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="S7" s="12"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="Y7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+    </row>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.75">
+      <c r="R8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="S8" s="13"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="Y8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+    </row>
+    <row r="9" spans="2:30" x14ac:dyDescent="0.75">
+      <c r="R9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="S9" s="12"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="Y9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z9" s="12"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+    </row>
+    <row r="10" spans="2:30" x14ac:dyDescent="0.75">
+      <c r="R10" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="S10" s="13"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="Y10" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="8"/>
+    </row>
+    <row r="11" spans="2:30" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="R11" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="S11" s="12"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="Y11" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Evaluate baseline on TrpB
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matou\Documents\mutagenesis-benchmarks\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B00F34F-CD68-4D37-B1DE-560A7AD10EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF47DE0-6AA0-4BD3-B4F8-651804F68E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="93">
   <si>
     <t>GFP</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -912,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AS17"/>
+  <dimension ref="B2:AS19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T7" workbookViewId="0">
-      <selection activeCell="AF16" sqref="AF16"/>
+    <sheetView tabSelected="1" topLeftCell="Q2" workbookViewId="0">
+      <selection activeCell="AA19" sqref="AA19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1895,25 +1898,54 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="18:31" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="17" spans="18:33" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="R17" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="S17" s="14"/>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15"/>
+      <c r="S17" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="T17" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="U17" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="V17" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="W17" s="15">
+        <v>0</v>
+      </c>
+      <c r="X17" s="15">
+        <v>80</v>
+      </c>
       <c r="Y17" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="Z17" s="14"/>
-      <c r="AA17" s="15"/>
-      <c r="AB17" s="15"/>
-      <c r="AC17" s="15"/>
-      <c r="AD17" s="15"/>
-      <c r="AE17" s="15"/>
+      <c r="Z17" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA17" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB17" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC17" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD17" s="15">
+        <v>2</v>
+      </c>
+      <c r="AE17" s="15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="18:33" x14ac:dyDescent="0.75">
+      <c r="AG19" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Evaluate FLIP cnn on non-zero data
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matou\Documents\mutagenesis-benchmarks\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF47DE0-6AA0-4BD3-B4F8-651804F68E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B28255-E41D-4B62-A82C-CB9E1BD4BB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="List3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="118">
   <si>
     <t>GFP</t>
   </si>
@@ -303,7 +304,82 @@
     <t>1</t>
   </si>
   <si>
-    <t>S</t>
+    <t>FLIP cnn</t>
+  </si>
+  <si>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>9.68</t>
+  </si>
+  <si>
+    <t>0.13</t>
+  </si>
+  <si>
+    <t>0.0010</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>without zero-fitness variants</t>
+  </si>
+  <si>
+    <t>FLIP ridge</t>
+  </si>
+  <si>
+    <t>GB1 = long sequences for cnn</t>
+  </si>
+  <si>
+    <t>0.005</t>
+  </si>
+  <si>
+    <t>0.0006</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>0.0005</t>
+  </si>
+  <si>
+    <t>0.008</t>
+  </si>
+  <si>
+    <t>mutated position only</t>
+  </si>
+  <si>
+    <t>mutated positions only</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2.0</t>
+  </si>
+  <si>
+    <t>0.004</t>
+  </si>
+  <si>
+    <t>0.04</t>
+  </si>
+  <si>
+    <t>0.12</t>
+  </si>
+  <si>
+    <t>0.0008</t>
+  </si>
+  <si>
+    <t>0.007</t>
+  </si>
+  <si>
+    <t>0.0002</t>
+  </si>
+  <si>
+    <t>5.45</t>
   </si>
 </sst>
 </file>
@@ -328,7 +404,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +425,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,7 +622,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -632,6 +714,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -915,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AS19"/>
+  <dimension ref="B2:AS24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q2" workbookViewId="0">
-      <selection activeCell="AA19" sqref="AA19"/>
+    <sheetView topLeftCell="AC8" workbookViewId="0">
+      <selection activeCell="AF19" sqref="AF19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -944,6 +1030,12 @@
       <c r="J2" t="s">
         <v>18</v>
       </c>
+      <c r="AF2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM2" s="9" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="3" spans="2:45" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="B3" s="3" t="s">
@@ -1759,192 +1851,379 @@
       <c r="AD12" s="9"/>
     </row>
     <row r="13" spans="2:45" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="R13" s="9" t="s">
+      <c r="AF13" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="Y13" s="9" t="s">
+      <c r="AM13" s="9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="2:45" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="R14" s="3" t="s">
+      <c r="AF14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="S14" s="7" t="s">
+      <c r="AG14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="T14" s="4" t="s">
+      <c r="AH14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="U14" s="4" t="s">
+      <c r="AI14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="V14" s="4" t="s">
+      <c r="AJ14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="W14" s="4" t="s">
+      <c r="AK14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="X14" s="5" t="s">
+      <c r="AL14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="Y14" s="3" t="s">
+      <c r="AM14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Z14" s="7" t="s">
+      <c r="AN14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AA14" s="4" t="s">
+      <c r="AO14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AB14" s="4" t="s">
+      <c r="AP14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AC14" s="4" t="s">
+      <c r="AQ14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AD14" s="4" t="s">
+      <c r="AR14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AE14" s="5" t="s">
+      <c r="AS14" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="2:45" x14ac:dyDescent="0.75">
-      <c r="R15" s="8" t="s">
+      <c r="AF15" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="S15" s="10" t="s">
+      <c r="AG15" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="T15" s="11" t="s">
+      <c r="AH15" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="U15" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="V15" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="W15" s="11">
+      <c r="AI15" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ15" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK15" s="11">
         <v>0</v>
       </c>
-      <c r="X15" s="11">
+      <c r="AL15" s="11">
         <v>79</v>
       </c>
-      <c r="Y15" s="28" t="s">
+      <c r="AM15" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="Z15" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA15" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB15" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC15" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD15" s="11">
+      <c r="AN15" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO15" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="AP15" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ15" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR15" s="11">
         <v>10</v>
       </c>
-      <c r="AE15" s="11">
+      <c r="AS15" s="11">
         <v>80</v>
       </c>
     </row>
     <row r="16" spans="2:45" x14ac:dyDescent="0.75">
-      <c r="R16" s="8" t="s">
+      <c r="AF16" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="S16" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="T16" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="U16" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="V16" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="W16" s="13">
+      <c r="AG16" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH16" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ16" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK16" s="13">
         <v>1</v>
       </c>
-      <c r="X16" s="13">
+      <c r="AL16" s="13">
         <v>80</v>
       </c>
-      <c r="Y16" s="28" t="s">
+      <c r="AM16" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="Z16" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA16" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB16" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC16" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD16" s="13">
+      <c r="AN16" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO16" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AP16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ16" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR16" s="13">
         <v>1</v>
       </c>
-      <c r="AE16" s="13">
+      <c r="AS16" s="13">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="18:33" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="R17" s="27" t="s">
+    <row r="17" spans="32:45" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="AF17" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="S17" s="14" t="s">
+      <c r="AG17" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="T17" s="15" t="s">
+      <c r="AH17" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="U17" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="V17" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="W17" s="15">
+      <c r="AI17" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ17" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK17" s="15">
         <v>0</v>
       </c>
-      <c r="X17" s="15">
+      <c r="AL17" s="15">
         <v>80</v>
       </c>
-      <c r="Y17" s="29" t="s">
+      <c r="AM17" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="Z17" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA17" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB17" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC17" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD17" s="15">
+      <c r="AN17" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO17" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="AP17" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ17" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR17" s="15">
         <v>2</v>
       </c>
-      <c r="AE17" s="15">
+      <c r="AS17" s="15">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="18:33" x14ac:dyDescent="0.75">
-      <c r="AG19" t="s">
-        <v>92</v>
+    <row r="19" spans="32:45" x14ac:dyDescent="0.75">
+      <c r="AF19" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM19" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="32:45" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="AF20" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM20" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="32:45" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="AF21" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG21" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH21" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI21" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ21" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK21" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL21" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM21" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN21" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO21" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="AP21" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="AQ21" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="AR21" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="AS21" s="34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="32:45" x14ac:dyDescent="0.75">
+      <c r="AF22" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG22" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH22" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI22" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ22" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK22" s="22">
+        <v>0</v>
+      </c>
+      <c r="AL22" s="22">
+        <v>80</v>
+      </c>
+      <c r="AM22" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN22" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO22" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP22" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ22" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR22" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="AS22" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="32:45" x14ac:dyDescent="0.75">
+      <c r="AF23" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG23" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH23" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI23" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ23" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK23" s="24">
+        <v>0</v>
+      </c>
+      <c r="AL23" s="24">
+        <v>80</v>
+      </c>
+      <c r="AM23" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN23" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="AO23" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="AP23" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ23" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR23" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="AS23" s="24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="32:45" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="AF24" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG24" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH24" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI24" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ24" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK24" s="26">
+        <v>2</v>
+      </c>
+      <c r="AL24" s="26">
+        <v>80</v>
+      </c>
+      <c r="AM24" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="AN24" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO24" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP24" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ24" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR24" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="AS24" s="26" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1953,4 +2232,1183 @@
     <ignoredError sqref="S4:S5 Z4:Z5" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03502709-4900-4203-8209-10B3E59F622F}">
+  <dimension ref="B2:AD35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="2" spans="2:30" x14ac:dyDescent="0.75">
+      <c r="B2" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q2" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="R2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="2:30" x14ac:dyDescent="0.75">
+      <c r="B3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="Q3" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="X3" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="2:30" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="X4" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:30" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q5" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="S5" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="T5" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="U5" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="V5" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="W5" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="X5" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z5" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA5" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB5" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC5" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD5" s="34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.75">
+      <c r="B6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="11">
+        <v>19</v>
+      </c>
+      <c r="H6" s="11">
+        <v>128</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="N6" s="11">
+        <v>0</v>
+      </c>
+      <c r="O6" s="11">
+        <v>128</v>
+      </c>
+      <c r="Q6" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="R6" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="S6" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="T6" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="U6" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="V6" s="22">
+        <v>8</v>
+      </c>
+      <c r="W6" s="22">
+        <v>128</v>
+      </c>
+      <c r="X6" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y6" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z6" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA6" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB6" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC6" s="22">
+        <v>4</v>
+      </c>
+      <c r="AD6" s="22">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.75">
+      <c r="B7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q7" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="R7" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="S7" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="T7" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="U7" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="V7" s="24">
+        <v>25</v>
+      </c>
+      <c r="W7" s="24">
+        <v>128</v>
+      </c>
+      <c r="X7" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y7" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z7" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA7" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB7" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC7" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD7" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="2:30" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B8" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="15">
+        <v>0</v>
+      </c>
+      <c r="H8" s="15">
+        <v>128</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="N8" s="15">
+        <v>0</v>
+      </c>
+      <c r="O8" s="15">
+        <v>128</v>
+      </c>
+      <c r="Q8" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="R8" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="S8" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="T8" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="U8" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="V8" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="W8" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="X8" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y8" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z8" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA8" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB8" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC8" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD8" s="26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="2:30" x14ac:dyDescent="0.75">
+      <c r="B11" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q11" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="R11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="2:30" x14ac:dyDescent="0.75">
+      <c r="B12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="Q12" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="X12" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="2:30" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B13" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q13" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="X13" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="2:30" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="U14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="W14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD14" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="2:30" x14ac:dyDescent="0.75">
+      <c r="B15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="11">
+        <v>22</v>
+      </c>
+      <c r="H15" s="11">
+        <v>128</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="M15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="N15" s="11">
+        <v>0</v>
+      </c>
+      <c r="O15" s="11">
+        <v>128</v>
+      </c>
+      <c r="Q15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="R15" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="S15" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="T15" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="U15" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="V15" s="11">
+        <v>125</v>
+      </c>
+      <c r="W15" s="11">
+        <v>128</v>
+      </c>
+      <c r="X15" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y15" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z15" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA15" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC15" s="11">
+        <v>12</v>
+      </c>
+      <c r="AD15" s="11">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="2:30" x14ac:dyDescent="0.75">
+      <c r="B16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="R16" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="S16" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="T16" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="U16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="V16" s="13">
+        <v>116</v>
+      </c>
+      <c r="W16" s="13">
+        <v>128</v>
+      </c>
+      <c r="X16" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y16" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z16" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC16" s="13">
+        <v>118</v>
+      </c>
+      <c r="AD16" s="13">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="2:30" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B17" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="15">
+        <v>0</v>
+      </c>
+      <c r="H17" s="15">
+        <v>128</v>
+      </c>
+      <c r="I17" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="L17" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="N17" s="15">
+        <v>0</v>
+      </c>
+      <c r="O17" s="15">
+        <v>128</v>
+      </c>
+      <c r="Q17" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="R17" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="S17" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="T17" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="U17" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="V17" s="15">
+        <v>0</v>
+      </c>
+      <c r="W17" s="15">
+        <v>128</v>
+      </c>
+      <c r="X17" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y17" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z17" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA17" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB17" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC17" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="15">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="2:30" x14ac:dyDescent="0.75">
+      <c r="Q20" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="R20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="2:30" x14ac:dyDescent="0.75">
+      <c r="Q21" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="X21" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="2:30" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="Q22" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="X22" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="2:30" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="Q23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="S23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="U23" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V23" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="W23" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="X23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y23" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB23" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC23" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD23" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="2:30" x14ac:dyDescent="0.75">
+      <c r="Q24" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="R24" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="S24" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="T24" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="U24" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="V24" s="11">
+        <v>107</v>
+      </c>
+      <c r="W24" s="11">
+        <v>128</v>
+      </c>
+      <c r="X24" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y24" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z24" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA24" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB24" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC24" s="11">
+        <v>2</v>
+      </c>
+      <c r="AD24" s="11">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="2:30" x14ac:dyDescent="0.75">
+      <c r="Q25" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="R25" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="S25" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="T25" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="U25" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="V25" s="13">
+        <v>33</v>
+      </c>
+      <c r="W25" s="13">
+        <v>128</v>
+      </c>
+      <c r="X25" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y25" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z25" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA25" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB25" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC25" s="13">
+        <v>88</v>
+      </c>
+      <c r="AD25" s="13">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="2:30" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="Q26" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="R26" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="S26" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="T26" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="U26" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="V26" s="15">
+        <v>2</v>
+      </c>
+      <c r="W26" s="15">
+        <v>128</v>
+      </c>
+      <c r="X26" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y26" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z26" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA26" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB26" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC26" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="15">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="2:30" x14ac:dyDescent="0.75">
+      <c r="Q29" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="R29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="2:30" x14ac:dyDescent="0.75">
+      <c r="Q30" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="X30" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="2:30" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="Q31" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="X31" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="2:30" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="Q32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R32" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="S32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T32" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="U32" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V32" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="W32" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="X32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y32" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA32" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB32" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC32" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD32" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="17:30" x14ac:dyDescent="0.75">
+      <c r="Q33" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="R33" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="S33" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="T33" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="U33" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="V33" s="11">
+        <v>125</v>
+      </c>
+      <c r="W33" s="11">
+        <v>128</v>
+      </c>
+      <c r="X33" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y33" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z33" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA33" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB33" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC33" s="11">
+        <v>12</v>
+      </c>
+      <c r="AD33" s="11">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="17:30" x14ac:dyDescent="0.75">
+      <c r="Q34" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="R34" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="S34" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="T34" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="U34" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="V34" s="13">
+        <v>116</v>
+      </c>
+      <c r="W34" s="13">
+        <v>128</v>
+      </c>
+      <c r="X34" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y34" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z34" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA34" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB34" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC34" s="13">
+        <v>118</v>
+      </c>
+      <c r="AD34" s="13">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="17:30" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="Q35" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="R35" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="S35" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="T35" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="U35" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="V35" s="15">
+        <v>0</v>
+      </c>
+      <c r="W35" s="15">
+        <v>128</v>
+      </c>
+      <c r="X35" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y35" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z35" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA35" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB35" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC35" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="15">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>